<commit_message>
[Update] Hud 일단 완성?
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excels/ItemSheets.xlsx
+++ b/Assets/Resources/Excels/ItemSheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\sparta_team\3D_TEAM12\Assets\Resources\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431EB4F5-BADC-45BB-9694-C36700F4EAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C68928-B3DF-4A2C-9995-3CAFDE130F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48315" yWindow="2820" windowWidth="19335" windowHeight="15285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemList" sheetId="1" r:id="rId1"/>
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39F50C1-EBAF-4FC6-84DD-C074EB80D8AB}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1824,7 +1824,7 @@
         <v>121</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1877,7 +1877,7 @@
         <v>122</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1930,7 +1930,7 @@
         <v>123</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>1.5</v>
@@ -1983,7 +1983,7 @@
         <v>121</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2036,7 +2036,7 @@
         <v>122</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2089,7 +2089,7 @@
         <v>123</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>1.5</v>
@@ -2142,7 +2142,7 @@
         <v>121</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2195,7 +2195,7 @@
         <v>122</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2248,7 +2248,7 @@
         <v>123</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>1.5</v>
@@ -2301,7 +2301,7 @@
         <v>121</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -2354,7 +2354,7 @@
         <v>122</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -2407,7 +2407,7 @@
         <v>123</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E13">
         <v>1.5</v>
@@ -2460,7 +2460,7 @@
         <v>124</v>
       </c>
       <c r="D14">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -2513,7 +2513,7 @@
         <v>125</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -2566,7 +2566,7 @@
         <v>126</v>
       </c>
       <c r="D16">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E16">
         <v>15</v>
@@ -2618,7 +2618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26320459-E182-4282-B0CD-FC10DCCE71E9}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>

</xml_diff>